<commit_message>
Updated Argent prices in Excel
</commit_message>
<xml_diff>
--- a/DataBI/Aluminium.xlsx
+++ b/DataBI/Aluminium.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B598"/>
+  <dimension ref="A1:B599"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A568" workbookViewId="0">
       <selection activeCell="J592" sqref="J592"/>
@@ -5225,6 +5225,18 @@
         </is>
       </c>
     </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>05/02/2025</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>2625,65</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>